<commit_message>
printer software: fix the communication and the baffle program
</commit_message>
<xml_diff>
--- a/BOM For Me.xlsx
+++ b/BOM For Me.xlsx
@@ -1166,7 +1166,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1271,11 +1271,11 @@
       </c>
       <c r="B8" s="13">
         <f ca="1">TODAY()</f>
-        <v>42810</v>
+        <v>42811</v>
       </c>
       <c r="C8" s="14">
         <f ca="1">NOW()</f>
-        <v>42810.708781597219</v>
+        <v>42811.71567060185</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="5"/>
@@ -1311,7 +1311,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="87">
         <f>ROW(A11) - ROW($A$10)</f>
         <v>1</v>
@@ -1322,7 +1322,7 @@
       <c r="E11" s="85"/>
       <c r="F11" s="85"/>
     </row>
-    <row r="12" spans="1:7" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="87">
         <f>ROW(A12) - ROW($A$10)</f>
         <v>2</v>
@@ -1333,7 +1333,7 @@
       <c r="E12" s="85"/>
       <c r="F12" s="85"/>
     </row>
-    <row r="13" spans="1:7" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="87">
         <f>ROW(A13) - ROW($A$10)</f>
         <v>3</v>

</xml_diff>